<commit_message>
i369--Jedi d6 suite update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_08_Jedi_D6.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_08_Jedi_D6.xlsx
@@ -5222,30 +5222,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{12D4C0FD-DD7F-423E-9D16-853FD11BF61F}" diskRevisions="1" revisionId="129" version="4">
-  <header guid="{565066FF-3387-4FED-BCB8-1D964CB6CA6E}" dateTime="2021-08-06T14:51:38" maxSheetId="5" userName="Jason Wang" r:id="rId1">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{692940B5-BE8D-4D6A-86D0-637A55FA3161}" dateTime="2021-08-06T14:55:47" maxSheetId="5" userName="Jason Wang" r:id="rId2" minRId="1" maxRId="2">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{3ACA605E-8DA3-4E12-8CE7-4284C7CC5DD8}" dateTime="2021-08-06T15:32:20" maxSheetId="5" userName="Jason Wang" r:id="rId3" minRId="3" maxRId="127">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
   <header guid="{12D4C0FD-DD7F-423E-9D16-853FD11BF61F}" dateTime="2021-08-06T15:32:25" maxSheetId="5" userName="Jason Wang" r:id="rId4">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5255,1365 +5231,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="1" sId="1" ref="A9:XFD9" action="insertRow"/>
-  <rcc rId="2" sId="1">
-    <nc r="A9" t="inlineStr">
-      <is>
-        <t>System</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="3" sId="2" ref="A6:XFD6" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A6:XFD6" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A6">
-        <v>4</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E6" t="inlineStr">
-        <is>
-          <t>00_primitive/00_common/04_CONFIG_LMMIB</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L6" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="S6" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE6" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="4" sId="2" ref="A94:XFD94" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A94:XFD94" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A94">
-        <v>93</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E94" t="inlineStr">
-        <is>
-          <t>00_primitive/06_DDR/12_IDDRX2DQ_30_mddrx2</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L94" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="S94" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE94" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="5" sId="2" ref="A95:XFD95" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A95:XFD95" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A95">
-        <v>95</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E95" t="inlineStr">
-        <is>
-          <t>00_primitive/06_DDR/14_IDDRX4DQ</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L95" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="S95" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE95" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="6" sId="2" ref="A100:XFD100" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A100:XFD100" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A100">
-        <v>101</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E100" t="inlineStr">
-        <is>
-          <t>00_primitive/06_DDR/20_ODDRX2DQS_30_mddrx2_r</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L100" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="S100" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE100" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="7" sId="2" ref="A101:XFD101" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A101:XFD101" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A101">
-        <v>103</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E101" t="inlineStr">
-        <is>
-          <t>00_primitive/06_DDR/22_ODDRX4DQ</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L101" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="S101" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE101" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="8" sId="2" ref="A101:XFD101" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A101:XFD101" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A101">
-        <v>104</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E101" t="inlineStr">
-        <is>
-          <t>00_primitive/06_DDR/23_ODDRX4DQS</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L101" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="S101" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE101" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="9" sId="2" ref="A104:XFD104" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A104:XFD104" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A104">
-        <v>108</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E104" t="inlineStr">
-        <is>
-          <t>00_primitive/06_DDR/27_TSHX2DQ_14_mddrx2</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="H104" t="inlineStr">
-        <is>
-          <t>silicon/04_Jedi/A_items/ARCs/ 05_DDR\DDR_timing\32_mddrx2_dq_dqs_ip</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L104" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="O104" t="inlineStr">
-        <is>
-          <t>cmd=--run-ipgen</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="S104" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE104" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="10" sId="2" ref="A104:XFD104" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A104:XFD104" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A104">
-        <v>109</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E104" t="inlineStr">
-        <is>
-          <t>00_primitive/06_DDR/28_TSHX2DQS_14_mddrx2</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L104" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="O104" t="inlineStr">
-        <is>
-          <t>cmd=--run-ipgen</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="S104" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE104" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="11" sId="2" ref="A104:XFD104" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A104:XFD104" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A104">
-        <v>110</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E104" t="inlineStr">
-        <is>
-          <t>00_primitive/06_DDR/29_TSHX4DQ</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L104" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="S104" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE104" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="12" sId="2" ref="A104:XFD104" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A104:XFD104" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="30" formatCode="@"/>
-        <protection locked="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" numFmtId="30">
-      <nc r="A104">
-        <v>111</v>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="E104" t="inlineStr">
-        <is>
-          <t>00_primitive/06_DDR/30_TSHX4DQS</t>
-        </is>
-      </nc>
-    </rcc>
-    <rfmt sheetId="2" sqref="L104" start="0" length="0">
-      <dxf>
-        <numFmt numFmtId="0" formatCode="General"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2">
-      <nc r="S104" t="inlineStr">
-        <is>
-          <t>primitive</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="2">
-      <nc r="AE104" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rcc rId="13" sId="2" numFmtId="30">
-    <oc r="A6">
-      <v>5</v>
-    </oc>
-    <nc r="A6">
-      <v>4</v>
-    </nc>
-  </rcc>
-  <rcc rId="14" sId="2" numFmtId="30">
-    <oc r="A7">
-      <v>6</v>
-    </oc>
-    <nc r="A7">
-      <v>5</v>
-    </nc>
-  </rcc>
-  <rcc rId="15" sId="2" numFmtId="30">
-    <oc r="A8">
-      <v>7</v>
-    </oc>
-    <nc r="A8">
-      <v>6</v>
-    </nc>
-  </rcc>
-  <rcc rId="16" sId="2" numFmtId="30">
-    <oc r="A9">
-      <v>8</v>
-    </oc>
-    <nc r="A9">
-      <v>7</v>
-    </nc>
-  </rcc>
-  <rcc rId="17" sId="2" numFmtId="30">
-    <oc r="A10">
-      <v>9</v>
-    </oc>
-    <nc r="A10">
-      <v>8</v>
-    </nc>
-  </rcc>
-  <rcc rId="18" sId="2" numFmtId="30">
-    <oc r="A11">
-      <v>10</v>
-    </oc>
-    <nc r="A11">
-      <v>9</v>
-    </nc>
-  </rcc>
-  <rcc rId="19" sId="2" numFmtId="30">
-    <oc r="A12">
-      <v>11</v>
-    </oc>
-    <nc r="A12">
-      <v>10</v>
-    </nc>
-  </rcc>
-  <rcc rId="20" sId="2" numFmtId="30">
-    <oc r="A13">
-      <v>12</v>
-    </oc>
-    <nc r="A13">
-      <v>11</v>
-    </nc>
-  </rcc>
-  <rcc rId="21" sId="2" numFmtId="30">
-    <oc r="A14">
-      <v>13</v>
-    </oc>
-    <nc r="A14">
-      <v>12</v>
-    </nc>
-  </rcc>
-  <rcc rId="22" sId="2" numFmtId="30">
-    <oc r="A15">
-      <v>14</v>
-    </oc>
-    <nc r="A15">
-      <v>13</v>
-    </nc>
-  </rcc>
-  <rcc rId="23" sId="2" numFmtId="30">
-    <oc r="A16">
-      <v>15</v>
-    </oc>
-    <nc r="A16">
-      <v>14</v>
-    </nc>
-  </rcc>
-  <rcc rId="24" sId="2" numFmtId="30">
-    <oc r="A17">
-      <v>16</v>
-    </oc>
-    <nc r="A17">
-      <v>15</v>
-    </nc>
-  </rcc>
-  <rcc rId="25" sId="2" numFmtId="30">
-    <oc r="A18">
-      <v>17</v>
-    </oc>
-    <nc r="A18">
-      <v>16</v>
-    </nc>
-  </rcc>
-  <rcc rId="26" sId="2" numFmtId="30">
-    <oc r="A19">
-      <v>18</v>
-    </oc>
-    <nc r="A19">
-      <v>17</v>
-    </nc>
-  </rcc>
-  <rcc rId="27" sId="2" numFmtId="30">
-    <oc r="A20">
-      <v>19</v>
-    </oc>
-    <nc r="A20">
-      <v>18</v>
-    </nc>
-  </rcc>
-  <rcc rId="28" sId="2" numFmtId="30">
-    <oc r="A21">
-      <v>20</v>
-    </oc>
-    <nc r="A21">
-      <v>19</v>
-    </nc>
-  </rcc>
-  <rcc rId="29" sId="2" numFmtId="30">
-    <oc r="A22">
-      <v>21</v>
-    </oc>
-    <nc r="A22">
-      <v>20</v>
-    </nc>
-  </rcc>
-  <rcc rId="30" sId="2" numFmtId="30">
-    <oc r="A23">
-      <v>22</v>
-    </oc>
-    <nc r="A23">
-      <v>21</v>
-    </nc>
-  </rcc>
-  <rcc rId="31" sId="2" numFmtId="30">
-    <oc r="A24">
-      <v>23</v>
-    </oc>
-    <nc r="A24">
-      <v>22</v>
-    </nc>
-  </rcc>
-  <rcc rId="32" sId="2" numFmtId="30">
-    <oc r="A25">
-      <v>24</v>
-    </oc>
-    <nc r="A25">
-      <v>23</v>
-    </nc>
-  </rcc>
-  <rcc rId="33" sId="2" numFmtId="30">
-    <oc r="A26">
-      <v>25</v>
-    </oc>
-    <nc r="A26">
-      <v>24</v>
-    </nc>
-  </rcc>
-  <rcc rId="34" sId="2" numFmtId="30">
-    <oc r="A27">
-      <v>26</v>
-    </oc>
-    <nc r="A27">
-      <v>25</v>
-    </nc>
-  </rcc>
-  <rcc rId="35" sId="2" numFmtId="30">
-    <oc r="A28">
-      <v>27</v>
-    </oc>
-    <nc r="A28">
-      <v>26</v>
-    </nc>
-  </rcc>
-  <rcc rId="36" sId="2" numFmtId="30">
-    <oc r="A29">
-      <v>28</v>
-    </oc>
-    <nc r="A29">
-      <v>27</v>
-    </nc>
-  </rcc>
-  <rcc rId="37" sId="2" numFmtId="30">
-    <oc r="A30">
-      <v>29</v>
-    </oc>
-    <nc r="A30">
-      <v>28</v>
-    </nc>
-  </rcc>
-  <rcc rId="38" sId="2" numFmtId="30">
-    <oc r="A31">
-      <v>30</v>
-    </oc>
-    <nc r="A31">
-      <v>29</v>
-    </nc>
-  </rcc>
-  <rcc rId="39" sId="2" numFmtId="30">
-    <oc r="A32">
-      <v>31</v>
-    </oc>
-    <nc r="A32">
-      <v>30</v>
-    </nc>
-  </rcc>
-  <rcc rId="40" sId="2" numFmtId="30">
-    <oc r="A33">
-      <v>32</v>
-    </oc>
-    <nc r="A33">
-      <v>31</v>
-    </nc>
-  </rcc>
-  <rcc rId="41" sId="2" numFmtId="30">
-    <oc r="A34">
-      <v>33</v>
-    </oc>
-    <nc r="A34">
-      <v>32</v>
-    </nc>
-  </rcc>
-  <rcc rId="42" sId="2" numFmtId="30">
-    <oc r="A35">
-      <v>34</v>
-    </oc>
-    <nc r="A35">
-      <v>33</v>
-    </nc>
-  </rcc>
-  <rcc rId="43" sId="2" numFmtId="30">
-    <oc r="A36">
-      <v>35</v>
-    </oc>
-    <nc r="A36">
-      <v>34</v>
-    </nc>
-  </rcc>
-  <rcc rId="44" sId="2" numFmtId="30">
-    <oc r="A37">
-      <v>36</v>
-    </oc>
-    <nc r="A37">
-      <v>35</v>
-    </nc>
-  </rcc>
-  <rcc rId="45" sId="2" numFmtId="30">
-    <oc r="A38">
-      <v>37</v>
-    </oc>
-    <nc r="A38">
-      <v>36</v>
-    </nc>
-  </rcc>
-  <rcc rId="46" sId="2" numFmtId="30">
-    <oc r="A39">
-      <v>38</v>
-    </oc>
-    <nc r="A39">
-      <v>37</v>
-    </nc>
-  </rcc>
-  <rcc rId="47" sId="2" numFmtId="30">
-    <oc r="A40">
-      <v>39</v>
-    </oc>
-    <nc r="A40">
-      <v>38</v>
-    </nc>
-  </rcc>
-  <rcc rId="48" sId="2" numFmtId="30">
-    <oc r="A41">
-      <v>40</v>
-    </oc>
-    <nc r="A41">
-      <v>39</v>
-    </nc>
-  </rcc>
-  <rcc rId="49" sId="2" numFmtId="30">
-    <oc r="A42">
-      <v>41</v>
-    </oc>
-    <nc r="A42">
-      <v>40</v>
-    </nc>
-  </rcc>
-  <rcc rId="50" sId="2" numFmtId="30">
-    <oc r="A43">
-      <v>42</v>
-    </oc>
-    <nc r="A43">
-      <v>41</v>
-    </nc>
-  </rcc>
-  <rcc rId="51" sId="2" numFmtId="30">
-    <oc r="A44">
-      <v>43</v>
-    </oc>
-    <nc r="A44">
-      <v>42</v>
-    </nc>
-  </rcc>
-  <rcc rId="52" sId="2" numFmtId="30">
-    <oc r="A45">
-      <v>44</v>
-    </oc>
-    <nc r="A45">
-      <v>43</v>
-    </nc>
-  </rcc>
-  <rcc rId="53" sId="2" numFmtId="30">
-    <oc r="A46">
-      <v>45</v>
-    </oc>
-    <nc r="A46">
-      <v>44</v>
-    </nc>
-  </rcc>
-  <rcc rId="54" sId="2" numFmtId="30">
-    <oc r="A47">
-      <v>46</v>
-    </oc>
-    <nc r="A47">
-      <v>45</v>
-    </nc>
-  </rcc>
-  <rcc rId="55" sId="2" numFmtId="30">
-    <oc r="A48">
-      <v>47</v>
-    </oc>
-    <nc r="A48">
-      <v>46</v>
-    </nc>
-  </rcc>
-  <rcc rId="56" sId="2" numFmtId="30">
-    <oc r="A49">
-      <v>48</v>
-    </oc>
-    <nc r="A49">
-      <v>47</v>
-    </nc>
-  </rcc>
-  <rcc rId="57" sId="2" numFmtId="30">
-    <oc r="A50">
-      <v>49</v>
-    </oc>
-    <nc r="A50">
-      <v>48</v>
-    </nc>
-  </rcc>
-  <rcc rId="58" sId="2" numFmtId="30">
-    <oc r="A51">
-      <v>50</v>
-    </oc>
-    <nc r="A51">
-      <v>49</v>
-    </nc>
-  </rcc>
-  <rcc rId="59" sId="2" numFmtId="30">
-    <oc r="A52">
-      <v>51</v>
-    </oc>
-    <nc r="A52">
-      <v>50</v>
-    </nc>
-  </rcc>
-  <rcc rId="60" sId="2" numFmtId="30">
-    <oc r="A53">
-      <v>52</v>
-    </oc>
-    <nc r="A53">
-      <v>51</v>
-    </nc>
-  </rcc>
-  <rcc rId="61" sId="2" numFmtId="30">
-    <oc r="A54">
-      <v>53</v>
-    </oc>
-    <nc r="A54">
-      <v>52</v>
-    </nc>
-  </rcc>
-  <rcc rId="62" sId="2" numFmtId="30">
-    <oc r="A55">
-      <v>54</v>
-    </oc>
-    <nc r="A55">
-      <v>53</v>
-    </nc>
-  </rcc>
-  <rcc rId="63" sId="2" numFmtId="30">
-    <oc r="A56">
-      <v>55</v>
-    </oc>
-    <nc r="A56">
-      <v>54</v>
-    </nc>
-  </rcc>
-  <rcc rId="64" sId="2" numFmtId="30">
-    <oc r="A57">
-      <v>56</v>
-    </oc>
-    <nc r="A57">
-      <v>55</v>
-    </nc>
-  </rcc>
-  <rcc rId="65" sId="2" numFmtId="30">
-    <oc r="A58">
-      <v>57</v>
-    </oc>
-    <nc r="A58">
-      <v>56</v>
-    </nc>
-  </rcc>
-  <rcc rId="66" sId="2" numFmtId="30">
-    <oc r="A59">
-      <v>58</v>
-    </oc>
-    <nc r="A59">
-      <v>57</v>
-    </nc>
-  </rcc>
-  <rcc rId="67" sId="2" numFmtId="30">
-    <oc r="A60">
-      <v>59</v>
-    </oc>
-    <nc r="A60">
-      <v>58</v>
-    </nc>
-  </rcc>
-  <rcc rId="68" sId="2" numFmtId="30">
-    <oc r="A61">
-      <v>60</v>
-    </oc>
-    <nc r="A61">
-      <v>59</v>
-    </nc>
-  </rcc>
-  <rcc rId="69" sId="2" numFmtId="30">
-    <oc r="A62">
-      <v>61</v>
-    </oc>
-    <nc r="A62">
-      <v>60</v>
-    </nc>
-  </rcc>
-  <rcc rId="70" sId="2" numFmtId="30">
-    <oc r="A63">
-      <v>62</v>
-    </oc>
-    <nc r="A63">
-      <v>61</v>
-    </nc>
-  </rcc>
-  <rcc rId="71" sId="2" numFmtId="30">
-    <oc r="A64">
-      <v>63</v>
-    </oc>
-    <nc r="A64">
-      <v>62</v>
-    </nc>
-  </rcc>
-  <rcc rId="72" sId="2" numFmtId="30">
-    <oc r="A65">
-      <v>64</v>
-    </oc>
-    <nc r="A65">
-      <v>63</v>
-    </nc>
-  </rcc>
-  <rcc rId="73" sId="2" numFmtId="30">
-    <oc r="A66">
-      <v>65</v>
-    </oc>
-    <nc r="A66">
-      <v>64</v>
-    </nc>
-  </rcc>
-  <rcc rId="74" sId="2" numFmtId="30">
-    <oc r="A67">
-      <v>66</v>
-    </oc>
-    <nc r="A67">
-      <v>65</v>
-    </nc>
-  </rcc>
-  <rcc rId="75" sId="2" numFmtId="30">
-    <oc r="A68">
-      <v>67</v>
-    </oc>
-    <nc r="A68">
-      <v>66</v>
-    </nc>
-  </rcc>
-  <rcc rId="76" sId="2" numFmtId="30">
-    <oc r="A69">
-      <v>68</v>
-    </oc>
-    <nc r="A69">
-      <v>67</v>
-    </nc>
-  </rcc>
-  <rcc rId="77" sId="2" numFmtId="30">
-    <oc r="A70">
-      <v>69</v>
-    </oc>
-    <nc r="A70">
-      <v>68</v>
-    </nc>
-  </rcc>
-  <rcc rId="78" sId="2" numFmtId="30">
-    <oc r="A71">
-      <v>70</v>
-    </oc>
-    <nc r="A71">
-      <v>69</v>
-    </nc>
-  </rcc>
-  <rcc rId="79" sId="2" numFmtId="30">
-    <oc r="A72">
-      <v>71</v>
-    </oc>
-    <nc r="A72">
-      <v>70</v>
-    </nc>
-  </rcc>
-  <rcc rId="80" sId="2" numFmtId="30">
-    <oc r="A73">
-      <v>72</v>
-    </oc>
-    <nc r="A73">
-      <v>71</v>
-    </nc>
-  </rcc>
-  <rcc rId="81" sId="2" numFmtId="30">
-    <oc r="A74">
-      <v>73</v>
-    </oc>
-    <nc r="A74">
-      <v>72</v>
-    </nc>
-  </rcc>
-  <rcc rId="82" sId="2" numFmtId="30">
-    <oc r="A75">
-      <v>74</v>
-    </oc>
-    <nc r="A75">
-      <v>73</v>
-    </nc>
-  </rcc>
-  <rcc rId="83" sId="2" numFmtId="30">
-    <oc r="A76">
-      <v>75</v>
-    </oc>
-    <nc r="A76">
-      <v>74</v>
-    </nc>
-  </rcc>
-  <rcc rId="84" sId="2" numFmtId="30">
-    <oc r="A77">
-      <v>76</v>
-    </oc>
-    <nc r="A77">
-      <v>75</v>
-    </nc>
-  </rcc>
-  <rcc rId="85" sId="2" numFmtId="30">
-    <oc r="A78">
-      <v>77</v>
-    </oc>
-    <nc r="A78">
-      <v>76</v>
-    </nc>
-  </rcc>
-  <rcc rId="86" sId="2" numFmtId="30">
-    <oc r="A79">
-      <v>78</v>
-    </oc>
-    <nc r="A79">
-      <v>77</v>
-    </nc>
-  </rcc>
-  <rcc rId="87" sId="2" numFmtId="30">
-    <oc r="A80">
-      <v>79</v>
-    </oc>
-    <nc r="A80">
-      <v>78</v>
-    </nc>
-  </rcc>
-  <rcc rId="88" sId="2" numFmtId="30">
-    <oc r="A81">
-      <v>80</v>
-    </oc>
-    <nc r="A81">
-      <v>79</v>
-    </nc>
-  </rcc>
-  <rcc rId="89" sId="2" numFmtId="30">
-    <oc r="A82">
-      <v>81</v>
-    </oc>
-    <nc r="A82">
-      <v>80</v>
-    </nc>
-  </rcc>
-  <rcc rId="90" sId="2" numFmtId="30">
-    <oc r="A83">
-      <v>82</v>
-    </oc>
-    <nc r="A83">
-      <v>81</v>
-    </nc>
-  </rcc>
-  <rcc rId="91" sId="2" numFmtId="30">
-    <oc r="A84">
-      <v>83</v>
-    </oc>
-    <nc r="A84">
-      <v>82</v>
-    </nc>
-  </rcc>
-  <rcc rId="92" sId="2" numFmtId="30">
-    <oc r="A85">
-      <v>84</v>
-    </oc>
-    <nc r="A85">
-      <v>83</v>
-    </nc>
-  </rcc>
-  <rcc rId="93" sId="2" numFmtId="30">
-    <oc r="A86">
-      <v>85</v>
-    </oc>
-    <nc r="A86">
-      <v>84</v>
-    </nc>
-  </rcc>
-  <rcc rId="94" sId="2" numFmtId="30">
-    <oc r="A87">
-      <v>86</v>
-    </oc>
-    <nc r="A87">
-      <v>85</v>
-    </nc>
-  </rcc>
-  <rcc rId="95" sId="2" numFmtId="30">
-    <oc r="A88">
-      <v>87</v>
-    </oc>
-    <nc r="A88">
-      <v>86</v>
-    </nc>
-  </rcc>
-  <rcc rId="96" sId="2" numFmtId="30">
-    <oc r="A89">
-      <v>88</v>
-    </oc>
-    <nc r="A89">
-      <v>87</v>
-    </nc>
-  </rcc>
-  <rcc rId="97" sId="2" numFmtId="30">
-    <oc r="A90">
-      <v>89</v>
-    </oc>
-    <nc r="A90">
-      <v>88</v>
-    </nc>
-  </rcc>
-  <rcc rId="98" sId="2" numFmtId="30">
-    <oc r="A91">
-      <v>90</v>
-    </oc>
-    <nc r="A91">
-      <v>89</v>
-    </nc>
-  </rcc>
-  <rcc rId="99" sId="2" numFmtId="30">
-    <oc r="A92">
-      <v>91</v>
-    </oc>
-    <nc r="A92">
-      <v>90</v>
-    </nc>
-  </rcc>
-  <rcc rId="100" sId="2" numFmtId="30">
-    <oc r="A93">
-      <v>92</v>
-    </oc>
-    <nc r="A93">
-      <v>91</v>
-    </nc>
-  </rcc>
-  <rcc rId="101" sId="2" numFmtId="30">
-    <oc r="A94">
-      <v>94</v>
-    </oc>
-    <nc r="A94">
-      <v>92</v>
-    </nc>
-  </rcc>
-  <rcc rId="102" sId="2" numFmtId="30">
-    <oc r="A95">
-      <v>96</v>
-    </oc>
-    <nc r="A95">
-      <v>93</v>
-    </nc>
-  </rcc>
-  <rcc rId="103" sId="2" numFmtId="30">
-    <oc r="A96">
-      <v>97</v>
-    </oc>
-    <nc r="A96">
-      <v>94</v>
-    </nc>
-  </rcc>
-  <rcc rId="104" sId="2" numFmtId="30">
-    <oc r="A97">
-      <v>98</v>
-    </oc>
-    <nc r="A97">
-      <v>95</v>
-    </nc>
-  </rcc>
-  <rcc rId="105" sId="2" numFmtId="30">
-    <oc r="A98">
-      <v>99</v>
-    </oc>
-    <nc r="A98">
-      <v>96</v>
-    </nc>
-  </rcc>
-  <rcc rId="106" sId="2" numFmtId="30">
-    <oc r="A99">
-      <v>100</v>
-    </oc>
-    <nc r="A99">
-      <v>97</v>
-    </nc>
-  </rcc>
-  <rcc rId="107" sId="2" numFmtId="30">
-    <oc r="A100">
-      <v>102</v>
-    </oc>
-    <nc r="A100">
-      <v>98</v>
-    </nc>
-  </rcc>
-  <rcc rId="108" sId="2" numFmtId="30">
-    <oc r="A101">
-      <v>105</v>
-    </oc>
-    <nc r="A101">
-      <v>99</v>
-    </nc>
-  </rcc>
-  <rcc rId="109" sId="2" numFmtId="30">
-    <oc r="A102">
-      <v>106</v>
-    </oc>
-    <nc r="A102">
-      <v>100</v>
-    </nc>
-  </rcc>
-  <rcc rId="110" sId="2" numFmtId="30">
-    <oc r="A103">
-      <v>107</v>
-    </oc>
-    <nc r="A103">
-      <v>101</v>
-    </nc>
-  </rcc>
-  <rcc rId="111" sId="2" numFmtId="30">
-    <oc r="A104">
-      <v>112</v>
-    </oc>
-    <nc r="A104">
-      <v>102</v>
-    </nc>
-  </rcc>
-  <rcc rId="112" sId="2" numFmtId="30">
-    <oc r="A105">
-      <v>113</v>
-    </oc>
-    <nc r="A105">
-      <v>103</v>
-    </nc>
-  </rcc>
-  <rcc rId="113" sId="2" numFmtId="30">
-    <oc r="A106">
-      <v>114</v>
-    </oc>
-    <nc r="A106">
-      <v>104</v>
-    </nc>
-  </rcc>
-  <rcc rId="114" sId="2" numFmtId="30">
-    <oc r="A107">
-      <v>115</v>
-    </oc>
-    <nc r="A107">
-      <v>105</v>
-    </nc>
-  </rcc>
-  <rcc rId="115" sId="2" numFmtId="30">
-    <oc r="A108">
-      <v>116</v>
-    </oc>
-    <nc r="A108">
-      <v>106</v>
-    </nc>
-  </rcc>
-  <rcc rId="116" sId="2" numFmtId="30">
-    <oc r="A109">
-      <v>117</v>
-    </oc>
-    <nc r="A109">
-      <v>107</v>
-    </nc>
-  </rcc>
-  <rcc rId="117" sId="2" numFmtId="30">
-    <oc r="A110">
-      <v>118</v>
-    </oc>
-    <nc r="A110">
-      <v>108</v>
-    </nc>
-  </rcc>
-  <rcc rId="118" sId="2" numFmtId="30">
-    <oc r="A111">
-      <v>119</v>
-    </oc>
-    <nc r="A111">
-      <v>109</v>
-    </nc>
-  </rcc>
-  <rcc rId="119" sId="2" numFmtId="30">
-    <oc r="A112">
-      <v>120</v>
-    </oc>
-    <nc r="A112">
-      <v>110</v>
-    </nc>
-  </rcc>
-  <rcc rId="120" sId="2" numFmtId="30">
-    <oc r="A113">
-      <v>121</v>
-    </oc>
-    <nc r="A113">
-      <v>111</v>
-    </nc>
-  </rcc>
-  <rcc rId="121" sId="2" numFmtId="30">
-    <oc r="A114">
-      <v>122</v>
-    </oc>
-    <nc r="A114">
-      <v>112</v>
-    </nc>
-  </rcc>
-  <rcc rId="122" sId="2" numFmtId="30">
-    <oc r="A115">
-      <v>123</v>
-    </oc>
-    <nc r="A115">
-      <v>113</v>
-    </nc>
-  </rcc>
-  <rcc rId="123" sId="2" numFmtId="30">
-    <oc r="A116">
-      <v>124</v>
-    </oc>
-    <nc r="A116">
-      <v>114</v>
-    </nc>
-  </rcc>
-  <rcc rId="124" sId="2" numFmtId="30">
-    <oc r="A117">
-      <v>125</v>
-    </oc>
-    <nc r="A117">
-      <v>115</v>
-    </nc>
-  </rcc>
-  <rcc rId="125" sId="2" numFmtId="30">
-    <oc r="A118">
-      <v>126</v>
-    </oc>
-    <nc r="A118">
-      <v>116</v>
-    </nc>
-  </rcc>
-  <rcc rId="126" sId="2" numFmtId="30">
-    <oc r="A119">
-      <v>127</v>
-    </oc>
-    <nc r="A119">
-      <v>117</v>
-    </nc>
-  </rcc>
-  <rcc rId="127" sId="2" numFmtId="30">
-    <oc r="A120">
-      <v>128</v>
-    </oc>
-    <nc r="A120">
-      <v>118</v>
-    </nc>
-  </rcc>
-  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>case!$A$2:$AE$120</formula>
-    <oldFormula>case!$A$2:$AE$120</oldFormula>
-  </rdn>
-  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>